<commit_message>
update Lorna's dates so p50 is floor of avg
</commit_message>
<xml_diff>
--- a/output/PWS_hatchery_eggtake_cleaned_20240410.xlsx
+++ b/output/PWS_hatchery_eggtake_cleaned_20240410.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Development\Wilson\Research\AHRP\Hemstrom pink salmon whole genome\Run timing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krshedd\Documents\R\PWS-Pink-WGR\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{E7FB4B5C-F54B-4D82-A116-837D417EC0C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B51951B-3885-4D2F-90F2-9B6D800B1E61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{320CBAE9-81BA-43EA-AF85-226A839AD941}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{320CBAE9-81BA-43EA-AF85-226A839AD941}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
@@ -969,7 +969,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L5" sqref="L5"/>
+      <selection pane="bottomLeft" activeCell="E155" sqref="E155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1162,7 +1162,7 @@
         <v>28359</v>
       </c>
       <c r="E5" s="3">
-        <v>28371</v>
+        <v>28370</v>
       </c>
       <c r="F5" s="3">
         <v>28382</v>
@@ -1170,8 +1170,8 @@
       <c r="G5" s="4">
         <v>234</v>
       </c>
-      <c r="H5" s="2">
-        <v>246</v>
+      <c r="H5" s="8">
+        <v>245</v>
       </c>
       <c r="I5" s="2">
         <v>257</v>
@@ -2292,15 +2292,12 @@
         <v>40063</v>
       </c>
       <c r="G37" s="7">
-        <f>D37-DATE(YEAR(D37),1,1)+1</f>
         <v>236</v>
       </c>
       <c r="H37" s="8">
-        <f>ROUND(((G37+I37)/2),0)</f>
         <v>243</v>
       </c>
       <c r="I37" s="7">
-        <f>F37-DATE(YEAR(F37),1,1)+1</f>
         <v>250</v>
       </c>
       <c r="J37" s="7">
@@ -5454,7 +5451,7 @@
         <v>30148</v>
       </c>
       <c r="E127" s="3">
-        <v>30159</v>
+        <v>30158</v>
       </c>
       <c r="F127" s="3">
         <v>30169</v>
@@ -5462,8 +5459,8 @@
       <c r="G127" s="4">
         <v>197</v>
       </c>
-      <c r="H127" s="2">
-        <v>208</v>
+      <c r="H127" s="8">
+        <v>207</v>
       </c>
       <c r="I127" s="2">
         <v>218</v>
@@ -6436,8 +6433,8 @@
       <c r="D155" s="5">
         <v>40384</v>
       </c>
-      <c r="E155" s="1">
-        <v>40397</v>
+      <c r="E155" s="5">
+        <v>40396</v>
       </c>
       <c r="F155" s="1">
         <v>40409</v>
@@ -6445,8 +6442,8 @@
       <c r="G155" s="8">
         <v>206</v>
       </c>
-      <c r="H155">
-        <v>219</v>
+      <c r="H155" s="8">
+        <v>218</v>
       </c>
       <c r="I155">
         <v>231</v>

</xml_diff>

<commit_message>
update duration to end - start + 1 (how many days did egg take take place)?
</commit_message>
<xml_diff>
--- a/output/PWS_hatchery_eggtake_cleaned_20240410.xlsx
+++ b/output/PWS_hatchery_eggtake_cleaned_20240410.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krshedd\Documents\R\PWS-Pink-WGR\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B51951B-3885-4D2F-90F2-9B6D800B1E61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE02C4D8-0A5A-4D48-AC23-5C154059720B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{320CBAE9-81BA-43EA-AF85-226A839AD941}"/>
   </bookViews>
@@ -965,11 +965,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46E80E18-1E6B-422F-AC97-431BA20C02DA}">
-  <dimension ref="A1:M167"/>
+  <dimension ref="A1:O167"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E155" sqref="E155"/>
+      <selection pane="bottomLeft" activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -987,7 +987,7 @@
     <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1056,7 +1056,7 @@
       <c r="I2" s="2">
         <v>254</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J2" s="7">
         <v>15</v>
       </c>
       <c r="K2" t="s">
@@ -1065,8 +1065,9 @@
       <c r="M2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O2" s="6"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1094,8 +1095,8 @@
       <c r="I3">
         <v>252</v>
       </c>
-      <c r="J3">
-        <v>21</v>
+      <c r="J3" s="8">
+        <v>22</v>
       </c>
       <c r="K3">
         <v>1552</v>
@@ -1106,8 +1107,9 @@
       <c r="M3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O3" s="6"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1135,8 +1137,8 @@
       <c r="I4">
         <v>265</v>
       </c>
-      <c r="J4">
-        <v>27</v>
+      <c r="J4" s="8">
+        <v>28</v>
       </c>
       <c r="K4">
         <v>1619</v>
@@ -1147,8 +1149,9 @@
       <c r="M4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O4" s="6"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1176,7 +1179,7 @@
       <c r="I5" s="2">
         <v>257</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="7">
         <v>24</v>
       </c>
       <c r="K5" t="s">
@@ -1185,8 +1188,9 @@
       <c r="M5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O5" s="6"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1214,14 +1218,15 @@
       <c r="I6">
         <v>244</v>
       </c>
-      <c r="J6">
-        <v>38</v>
+      <c r="J6" s="8">
+        <v>39</v>
       </c>
       <c r="K6">
         <v>1782</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O6" s="6"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1249,14 +1254,15 @@
       <c r="I7">
         <v>257</v>
       </c>
-      <c r="J7">
-        <v>46</v>
+      <c r="J7" s="8">
+        <v>47</v>
       </c>
       <c r="K7">
         <v>1660</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O7" s="6"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1284,14 +1290,15 @@
       <c r="I8">
         <v>239</v>
       </c>
-      <c r="J8">
-        <v>2</v>
+      <c r="J8" s="8">
+        <v>3</v>
       </c>
       <c r="K8">
         <v>1670</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O8" s="6"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1319,14 +1326,15 @@
       <c r="I9">
         <v>261</v>
       </c>
-      <c r="J9">
-        <v>23</v>
+      <c r="J9" s="8">
+        <v>24</v>
       </c>
       <c r="K9">
         <v>1675</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O9" s="6"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1354,14 +1362,15 @@
       <c r="I10">
         <v>264</v>
       </c>
-      <c r="J10">
-        <v>17</v>
+      <c r="J10" s="8">
+        <v>18</v>
       </c>
       <c r="K10">
         <v>1565</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O10" s="6"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1389,14 +1398,15 @@
       <c r="I11">
         <v>259</v>
       </c>
-      <c r="J11">
-        <v>18</v>
+      <c r="J11" s="8">
+        <v>19</v>
       </c>
       <c r="K11">
         <v>1618</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O11" s="6"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1424,14 +1434,15 @@
       <c r="I12">
         <v>258</v>
       </c>
-      <c r="J12">
-        <v>20</v>
+      <c r="J12" s="8">
+        <v>21</v>
       </c>
       <c r="K12">
         <v>1678</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O12" s="6"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1459,14 +1470,15 @@
       <c r="I13">
         <v>261</v>
       </c>
-      <c r="J13">
-        <v>23</v>
+      <c r="J13" s="8">
+        <v>24</v>
       </c>
       <c r="K13">
         <v>1519</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O13" s="6"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -1494,14 +1506,15 @@
       <c r="I14">
         <v>261</v>
       </c>
-      <c r="J14">
-        <v>23</v>
+      <c r="J14" s="8">
+        <v>24</v>
       </c>
       <c r="K14">
         <v>1641</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O14" s="6"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -1529,14 +1542,15 @@
       <c r="I15">
         <v>260</v>
       </c>
-      <c r="J15">
-        <v>21</v>
+      <c r="J15" s="8">
+        <v>22</v>
       </c>
       <c r="K15">
         <v>1647</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O15" s="6"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -1564,14 +1578,15 @@
       <c r="I16">
         <v>263</v>
       </c>
-      <c r="J16">
-        <v>27</v>
+      <c r="J16" s="8">
+        <v>28</v>
       </c>
       <c r="K16">
         <v>1626</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O16" s="6"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -1599,14 +1614,15 @@
       <c r="I17">
         <v>250</v>
       </c>
-      <c r="J17">
-        <v>13</v>
+      <c r="J17" s="8">
+        <v>14</v>
       </c>
       <c r="K17">
         <v>1565</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O17" s="6"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -1634,14 +1650,15 @@
       <c r="I18">
         <v>256</v>
       </c>
-      <c r="J18">
-        <v>20</v>
+      <c r="J18" s="8">
+        <v>21</v>
       </c>
       <c r="K18">
         <v>1668</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O18" s="6"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -1669,14 +1686,15 @@
       <c r="I19">
         <v>256</v>
       </c>
-      <c r="J19">
-        <v>19</v>
+      <c r="J19" s="8">
+        <v>20</v>
       </c>
       <c r="K19">
         <v>1423</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O19" s="6"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -1704,14 +1722,15 @@
       <c r="I20">
         <v>259</v>
       </c>
-      <c r="J20">
-        <v>22</v>
+      <c r="J20" s="8">
+        <v>23</v>
       </c>
       <c r="K20">
         <v>1767</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O20" s="6"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -1739,14 +1758,15 @@
       <c r="I21">
         <v>256</v>
       </c>
-      <c r="J21">
-        <v>23</v>
+      <c r="J21" s="8">
+        <v>24</v>
       </c>
       <c r="K21">
         <v>1475</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O21" s="6"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -1774,14 +1794,15 @@
       <c r="I22">
         <v>253</v>
       </c>
-      <c r="J22">
-        <v>18</v>
+      <c r="J22" s="8">
+        <v>19</v>
       </c>
       <c r="K22">
         <v>1807</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O22" s="6"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>11</v>
       </c>
@@ -1809,14 +1830,15 @@
       <c r="I23">
         <v>255</v>
       </c>
-      <c r="J23">
-        <v>20</v>
+      <c r="J23" s="8">
+        <v>21</v>
       </c>
       <c r="K23" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O23" s="6"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>11</v>
       </c>
@@ -1850,8 +1872,9 @@
       <c r="K24">
         <v>1506</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O24" s="6"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>11</v>
       </c>
@@ -1885,8 +1908,9 @@
       <c r="K25" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O25" s="6"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>11</v>
       </c>
@@ -1914,14 +1938,15 @@
       <c r="I26">
         <v>260</v>
       </c>
-      <c r="J26">
-        <v>24</v>
+      <c r="J26" s="8">
+        <v>25</v>
       </c>
       <c r="K26">
         <v>1554</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O26" s="6"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>11</v>
       </c>
@@ -1949,14 +1974,15 @@
       <c r="I27">
         <v>266</v>
       </c>
-      <c r="J27">
-        <v>26</v>
+      <c r="J27" s="8">
+        <v>27</v>
       </c>
       <c r="K27">
         <v>1226</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O27" s="6"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>11</v>
       </c>
@@ -1984,14 +2010,15 @@
       <c r="I28">
         <v>261</v>
       </c>
-      <c r="J28">
-        <v>20</v>
+      <c r="J28" s="8">
+        <v>21</v>
       </c>
       <c r="K28">
         <v>1583</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O28" s="6"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>11</v>
       </c>
@@ -2019,14 +2046,15 @@
       <c r="I29">
         <v>259</v>
       </c>
-      <c r="J29">
-        <v>20</v>
+      <c r="J29" s="8">
+        <v>21</v>
       </c>
       <c r="K29">
         <v>1454</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O29" s="6"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>11</v>
       </c>
@@ -2054,14 +2082,15 @@
       <c r="I30">
         <v>259</v>
       </c>
-      <c r="J30">
-        <v>19</v>
+      <c r="J30" s="8">
+        <v>20</v>
       </c>
       <c r="K30">
         <v>1564</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O30" s="6"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>11</v>
       </c>
@@ -2089,14 +2118,15 @@
       <c r="I31">
         <v>257</v>
       </c>
-      <c r="J31">
-        <v>19</v>
+      <c r="J31" s="8">
+        <v>20</v>
       </c>
       <c r="K31">
         <v>1462</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O31" s="6"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>11</v>
       </c>
@@ -2124,14 +2154,15 @@
       <c r="I32">
         <v>268</v>
       </c>
-      <c r="J32">
-        <v>28</v>
+      <c r="J32" s="8">
+        <v>29</v>
       </c>
       <c r="K32">
         <v>1530</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O32" s="6"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>11</v>
       </c>
@@ -2159,14 +2190,15 @@
       <c r="I33">
         <v>261</v>
       </c>
-      <c r="J33">
-        <v>26</v>
+      <c r="J33" s="8">
+        <v>27</v>
       </c>
       <c r="K33">
         <v>1436</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O33" s="6"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>11</v>
       </c>
@@ -2194,14 +2226,15 @@
       <c r="I34">
         <v>262</v>
       </c>
-      <c r="J34">
-        <v>22</v>
+      <c r="J34" s="8">
+        <v>23</v>
       </c>
       <c r="K34">
         <v>1662</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O34" s="6"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>11</v>
       </c>
@@ -2229,14 +2262,15 @@
       <c r="I35">
         <v>255</v>
       </c>
-      <c r="J35">
-        <v>16</v>
+      <c r="J35" s="8">
+        <v>17</v>
       </c>
       <c r="K35">
         <v>1481</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O35" s="6"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>11</v>
       </c>
@@ -2264,14 +2298,15 @@
       <c r="I36">
         <v>254</v>
       </c>
-      <c r="J36">
-        <v>16</v>
+      <c r="J36" s="8">
+        <v>17</v>
       </c>
       <c r="K36">
         <v>1455</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O36" s="6"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>11</v>
       </c>
@@ -2301,14 +2336,14 @@
         <v>250</v>
       </c>
       <c r="J37" s="7">
-        <f>I37-G37+1</f>
         <v>15</v>
       </c>
       <c r="K37">
         <v>1504</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O37" s="6"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>11</v>
       </c>
@@ -2336,14 +2371,15 @@
       <c r="I38">
         <v>247</v>
       </c>
-      <c r="J38">
-        <v>11</v>
+      <c r="J38" s="8">
+        <v>12</v>
       </c>
       <c r="K38">
         <v>1629</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O38" s="6"/>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>11</v>
       </c>
@@ -2371,14 +2407,15 @@
       <c r="I39">
         <v>247</v>
       </c>
-      <c r="J39">
-        <v>11</v>
+      <c r="J39" s="8">
+        <v>12</v>
       </c>
       <c r="K39">
         <v>1451</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O39" s="6"/>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>11</v>
       </c>
@@ -2406,14 +2443,15 @@
       <c r="I40">
         <v>251</v>
       </c>
-      <c r="J40">
-        <v>14</v>
+      <c r="J40" s="8">
+        <v>15</v>
       </c>
       <c r="K40">
         <v>1633</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O40" s="6"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>11</v>
       </c>
@@ -2441,14 +2479,15 @@
       <c r="I41">
         <v>247</v>
       </c>
-      <c r="J41">
-        <v>14</v>
+      <c r="J41" s="8">
+        <v>15</v>
       </c>
       <c r="K41">
         <v>1378</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O41" s="6"/>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>11</v>
       </c>
@@ -2476,14 +2515,15 @@
       <c r="I42">
         <v>248</v>
       </c>
-      <c r="J42">
-        <v>15</v>
+      <c r="J42" s="8">
+        <v>16</v>
       </c>
       <c r="K42">
         <v>1516</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O42" s="6"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>11</v>
       </c>
@@ -2511,14 +2551,15 @@
       <c r="I43">
         <v>249</v>
       </c>
-      <c r="J43">
-        <v>12</v>
+      <c r="J43" s="8">
+        <v>13</v>
       </c>
       <c r="K43">
         <v>1196</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O43" s="6"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>11</v>
       </c>
@@ -2546,14 +2587,15 @@
       <c r="I44">
         <v>258</v>
       </c>
-      <c r="J44">
-        <v>25</v>
+      <c r="J44" s="8">
+        <v>26</v>
       </c>
       <c r="K44">
         <v>1815</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O44" s="6"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>11</v>
       </c>
@@ -2581,14 +2623,15 @@
       <c r="I45">
         <v>257</v>
       </c>
-      <c r="J45">
-        <v>18</v>
+      <c r="J45" s="8">
+        <v>19</v>
       </c>
       <c r="K45">
         <v>1336</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O45" s="6"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>11</v>
       </c>
@@ -2616,14 +2659,15 @@
       <c r="I46">
         <v>248</v>
       </c>
-      <c r="J46">
-        <v>11</v>
+      <c r="J46" s="8">
+        <v>12</v>
       </c>
       <c r="K46">
         <v>1549</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O46" s="6"/>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>11</v>
       </c>
@@ -2651,14 +2695,15 @@
       <c r="I47">
         <v>257</v>
       </c>
-      <c r="J47">
-        <v>16</v>
+      <c r="J47" s="8">
+        <v>17</v>
       </c>
       <c r="K47">
         <v>1236</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O47" s="6"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>11</v>
       </c>
@@ -2686,14 +2731,15 @@
       <c r="I48">
         <v>255</v>
       </c>
-      <c r="J48">
-        <v>17</v>
+      <c r="J48" s="8">
+        <v>18</v>
       </c>
       <c r="K48">
         <v>1427</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O48" s="6"/>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>11</v>
       </c>
@@ -2721,14 +2767,15 @@
       <c r="I49">
         <v>249</v>
       </c>
-      <c r="J49">
-        <v>11</v>
+      <c r="J49" s="8">
+        <v>12</v>
       </c>
       <c r="K49">
         <v>1306</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O49" s="6"/>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>15</v>
       </c>
@@ -2756,14 +2803,15 @@
       <c r="I50" s="2">
         <v>259</v>
       </c>
-      <c r="J50" s="4">
+      <c r="J50" s="7">
         <v>25</v>
       </c>
       <c r="K50" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O50" s="6"/>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>15</v>
       </c>
@@ -2791,14 +2839,15 @@
       <c r="I51">
         <v>255</v>
       </c>
-      <c r="J51">
-        <v>21</v>
+      <c r="J51" s="8">
+        <v>22</v>
       </c>
       <c r="K51">
         <v>1736</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O51" s="6"/>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>15</v>
       </c>
@@ -2826,14 +2875,15 @@
       <c r="I52">
         <v>257</v>
       </c>
-      <c r="J52">
-        <v>23</v>
+      <c r="J52" s="8">
+        <v>24</v>
       </c>
       <c r="K52">
         <v>1513</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O52" s="6"/>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>15</v>
       </c>
@@ -2861,14 +2911,15 @@
       <c r="I53">
         <v>257</v>
       </c>
-      <c r="J53">
-        <v>21</v>
+      <c r="J53" s="8">
+        <v>22</v>
       </c>
       <c r="K53">
         <v>1528</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O53" s="6"/>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>15</v>
       </c>
@@ -2896,14 +2947,15 @@
       <c r="I54">
         <v>258</v>
       </c>
-      <c r="J54">
-        <v>26</v>
+      <c r="J54" s="8">
+        <v>27</v>
       </c>
       <c r="K54">
         <v>1495</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O54" s="6"/>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>15</v>
       </c>
@@ -2931,14 +2983,15 @@
       <c r="I55">
         <v>250</v>
       </c>
-      <c r="J55">
-        <v>16</v>
+      <c r="J55" s="8">
+        <v>17</v>
       </c>
       <c r="K55">
         <v>1515</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O55" s="6"/>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>15</v>
       </c>
@@ -2966,14 +3019,15 @@
       <c r="I56">
         <v>259</v>
       </c>
-      <c r="J56">
-        <v>20</v>
+      <c r="J56" s="8">
+        <v>21</v>
       </c>
       <c r="K56">
         <v>1111</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O56" s="6"/>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>15</v>
       </c>
@@ -3001,14 +3055,15 @@
       <c r="I57">
         <v>254</v>
       </c>
-      <c r="J57">
-        <v>16</v>
+      <c r="J57" s="8">
+        <v>17</v>
       </c>
       <c r="K57">
         <v>1555</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O57" s="6"/>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>15</v>
       </c>
@@ -3036,14 +3091,15 @@
       <c r="I58">
         <v>263</v>
       </c>
-      <c r="J58">
-        <v>24</v>
+      <c r="J58" s="8">
+        <v>25</v>
       </c>
       <c r="K58">
         <v>1453</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O58" s="6"/>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>15</v>
       </c>
@@ -3071,14 +3127,15 @@
       <c r="I59">
         <v>256</v>
       </c>
-      <c r="J59">
-        <v>17</v>
+      <c r="J59" s="8">
+        <v>18</v>
       </c>
       <c r="K59">
         <v>1466</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O59" s="6"/>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>15</v>
       </c>
@@ -3106,14 +3163,15 @@
       <c r="I60">
         <v>249</v>
       </c>
-      <c r="J60">
-        <v>16</v>
+      <c r="J60" s="8">
+        <v>17</v>
       </c>
       <c r="K60">
         <v>1559</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O60" s="6"/>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>15</v>
       </c>
@@ -3141,14 +3199,15 @@
       <c r="I61">
         <v>259</v>
       </c>
-      <c r="J61">
-        <v>20</v>
+      <c r="J61" s="8">
+        <v>21</v>
       </c>
       <c r="K61">
         <v>1426</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O61" s="6"/>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>15</v>
       </c>
@@ -3176,14 +3235,15 @@
       <c r="I62">
         <v>259</v>
       </c>
-      <c r="J62">
-        <v>31</v>
+      <c r="J62" s="8">
+        <v>32</v>
       </c>
       <c r="K62">
         <v>1249</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O62" s="6"/>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>15</v>
       </c>
@@ -3211,14 +3271,15 @@
       <c r="I63">
         <v>251</v>
       </c>
-      <c r="J63">
-        <v>14</v>
+      <c r="J63" s="8">
+        <v>15</v>
       </c>
       <c r="K63">
         <v>1606</v>
       </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O63" s="6"/>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>15</v>
       </c>
@@ -3246,14 +3307,15 @@
       <c r="I64">
         <v>251</v>
       </c>
-      <c r="J64">
-        <v>15</v>
+      <c r="J64" s="8">
+        <v>16</v>
       </c>
       <c r="K64">
         <v>1369</v>
       </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O64" s="6"/>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>15</v>
       </c>
@@ -3281,14 +3343,15 @@
       <c r="I65">
         <v>254</v>
       </c>
-      <c r="J65">
-        <v>17</v>
+      <c r="J65" s="8">
+        <v>18</v>
       </c>
       <c r="K65">
         <v>1559</v>
       </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O65" s="6"/>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>15</v>
       </c>
@@ -3316,14 +3379,15 @@
       <c r="I66">
         <v>249</v>
       </c>
-      <c r="J66">
-        <v>13</v>
+      <c r="J66" s="8">
+        <v>14</v>
       </c>
       <c r="K66">
         <v>1290</v>
       </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O66" s="6"/>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>15</v>
       </c>
@@ -3351,14 +3415,15 @@
       <c r="I67">
         <v>246</v>
       </c>
-      <c r="J67">
-        <v>10</v>
+      <c r="J67" s="8">
+        <v>11</v>
       </c>
       <c r="K67">
         <v>1477</v>
       </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O67" s="6"/>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>15</v>
       </c>
@@ -3386,14 +3451,15 @@
       <c r="I68">
         <v>249</v>
       </c>
-      <c r="J68">
-        <v>12</v>
+      <c r="J68" s="8">
+        <v>13</v>
       </c>
       <c r="K68">
         <v>1224</v>
       </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O68" s="6"/>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>15</v>
       </c>
@@ -3421,14 +3487,15 @@
       <c r="I69">
         <v>247</v>
       </c>
-      <c r="J69">
-        <v>10</v>
+      <c r="J69" s="8">
+        <v>11</v>
       </c>
       <c r="K69">
         <v>1620</v>
       </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O69" s="6"/>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>15</v>
       </c>
@@ -3456,14 +3523,15 @@
       <c r="I70">
         <v>247</v>
       </c>
-      <c r="J70">
-        <v>15</v>
+      <c r="J70" s="8">
+        <v>16</v>
       </c>
       <c r="K70">
         <v>1102</v>
       </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O70" s="6"/>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>15</v>
       </c>
@@ -3491,14 +3559,15 @@
       <c r="I71">
         <v>242</v>
       </c>
-      <c r="J71">
-        <v>10</v>
+      <c r="J71" s="8">
+        <v>11</v>
       </c>
       <c r="K71">
         <v>1305</v>
       </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O71" s="6"/>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>15</v>
       </c>
@@ -3526,14 +3595,15 @@
       <c r="I72">
         <v>253</v>
       </c>
-      <c r="J72">
-        <v>17</v>
+      <c r="J72" s="8">
+        <v>18</v>
       </c>
       <c r="K72">
         <v>1028</v>
       </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O72" s="6"/>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>15</v>
       </c>
@@ -3561,14 +3631,15 @@
       <c r="I73">
         <v>253</v>
       </c>
-      <c r="J73">
-        <v>21</v>
+      <c r="J73" s="8">
+        <v>22</v>
       </c>
       <c r="K73">
         <v>1431</v>
       </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O73" s="6"/>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>15</v>
       </c>
@@ -3596,14 +3667,15 @@
       <c r="I74">
         <v>250</v>
       </c>
-      <c r="J74">
-        <v>11</v>
+      <c r="J74" s="8">
+        <v>12</v>
       </c>
       <c r="K74">
         <v>1382</v>
       </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O74" s="6"/>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>15</v>
       </c>
@@ -3631,14 +3703,15 @@
       <c r="I75">
         <v>251</v>
       </c>
-      <c r="J75">
-        <v>16</v>
+      <c r="J75" s="8">
+        <v>17</v>
       </c>
       <c r="K75">
         <v>1367</v>
       </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O75" s="6"/>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>15</v>
       </c>
@@ -3666,14 +3739,15 @@
       <c r="I76">
         <v>258</v>
       </c>
-      <c r="J76">
-        <v>20</v>
+      <c r="J76" s="8">
+        <v>21</v>
       </c>
       <c r="K76">
         <v>1226</v>
       </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O76" s="6"/>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>15</v>
       </c>
@@ -3701,14 +3775,15 @@
       <c r="I77">
         <v>251</v>
       </c>
-      <c r="J77">
-        <v>17</v>
+      <c r="J77" s="8">
+        <v>18</v>
       </c>
       <c r="K77">
         <v>1395</v>
       </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O77" s="6"/>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>15</v>
       </c>
@@ -3736,14 +3811,15 @@
       <c r="I78">
         <v>251</v>
       </c>
-      <c r="J78">
-        <v>16</v>
+      <c r="J78" s="8">
+        <v>17</v>
       </c>
       <c r="K78">
         <v>1310</v>
       </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O78" s="6"/>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>16</v>
       </c>
@@ -3777,8 +3853,9 @@
       <c r="K79" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O79" s="6"/>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>16</v>
       </c>
@@ -3812,8 +3889,9 @@
       <c r="K80" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O80" s="6"/>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>16</v>
       </c>
@@ -3847,8 +3925,9 @@
       <c r="K81" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O81" s="6"/>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>16</v>
       </c>
@@ -3885,8 +3964,9 @@
       <c r="M82">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O82" s="6"/>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>16</v>
       </c>
@@ -3923,8 +4003,9 @@
       <c r="M83">
         <v>1</v>
       </c>
-    </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O83" s="6"/>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>16</v>
       </c>
@@ -3961,8 +4042,9 @@
       <c r="M84">
         <v>1</v>
       </c>
-    </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O84" s="6"/>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>16</v>
       </c>
@@ -3996,8 +4078,9 @@
       <c r="K85" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O85" s="6"/>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>16</v>
       </c>
@@ -4031,8 +4114,9 @@
       <c r="K86" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O86" s="6"/>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>16</v>
       </c>
@@ -4066,8 +4150,9 @@
       <c r="K87" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O87" s="6"/>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>16</v>
       </c>
@@ -4101,8 +4186,9 @@
       <c r="K88" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O88" s="6"/>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>16</v>
       </c>
@@ -4136,8 +4222,9 @@
       <c r="K89" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O89" s="6"/>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>16</v>
       </c>
@@ -4171,8 +4258,9 @@
       <c r="K90" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O90" s="6"/>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>16</v>
       </c>
@@ -4206,8 +4294,9 @@
       <c r="K91" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O91" s="6"/>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>16</v>
       </c>
@@ -4235,14 +4324,15 @@
       <c r="I92">
         <v>269</v>
       </c>
-      <c r="J92">
-        <v>29</v>
+      <c r="J92" s="8">
+        <v>30</v>
       </c>
       <c r="K92">
         <v>1674</v>
       </c>
-    </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O92" s="6"/>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>16</v>
       </c>
@@ -4270,14 +4360,15 @@
       <c r="I93">
         <v>261</v>
       </c>
-      <c r="J93">
-        <v>26</v>
+      <c r="J93" s="8">
+        <v>27</v>
       </c>
       <c r="K93">
         <v>1610</v>
       </c>
-    </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O93" s="6"/>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>16</v>
       </c>
@@ -4305,14 +4396,15 @@
       <c r="I94">
         <v>257</v>
       </c>
-      <c r="J94">
-        <v>20</v>
+      <c r="J94" s="8">
+        <v>21</v>
       </c>
       <c r="K94">
         <v>1528</v>
       </c>
-    </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O94" s="6"/>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>16</v>
       </c>
@@ -4340,14 +4432,15 @@
       <c r="I95">
         <v>257</v>
       </c>
-      <c r="J95">
-        <v>21</v>
+      <c r="J95" s="8">
+        <v>22</v>
       </c>
       <c r="K95">
         <v>1315</v>
       </c>
-    </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O95" s="6"/>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>16</v>
       </c>
@@ -4375,14 +4468,15 @@
       <c r="I96">
         <v>257</v>
       </c>
-      <c r="J96">
-        <v>20</v>
+      <c r="J96" s="8">
+        <v>21</v>
       </c>
       <c r="K96">
         <v>1752</v>
       </c>
-    </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O96" s="6"/>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>16</v>
       </c>
@@ -4410,14 +4504,15 @@
       <c r="I97">
         <v>258</v>
       </c>
-      <c r="J97">
-        <v>22</v>
+      <c r="J97" s="8">
+        <v>23</v>
       </c>
       <c r="K97">
         <v>1438</v>
       </c>
-    </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O97" s="6"/>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>16</v>
       </c>
@@ -4445,14 +4540,15 @@
       <c r="I98">
         <v>258</v>
       </c>
-      <c r="J98">
-        <v>22</v>
+      <c r="J98" s="8">
+        <v>23</v>
       </c>
       <c r="K98">
         <v>1671</v>
       </c>
-    </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O98" s="6"/>
+    </row>
+    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>16</v>
       </c>
@@ -4480,14 +4576,15 @@
       <c r="I99">
         <v>260</v>
       </c>
-      <c r="J99">
-        <v>17</v>
+      <c r="J99" s="8">
+        <v>18</v>
       </c>
       <c r="K99">
         <v>1500</v>
       </c>
-    </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O99" s="6"/>
+    </row>
+    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>16</v>
       </c>
@@ -4515,14 +4612,15 @@
       <c r="I100">
         <v>259</v>
       </c>
-      <c r="J100">
-        <v>18</v>
+      <c r="J100" s="8">
+        <v>19</v>
       </c>
       <c r="K100">
         <v>1588</v>
       </c>
-    </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O100" s="6"/>
+    </row>
+    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>16</v>
       </c>
@@ -4550,14 +4648,15 @@
       <c r="I101">
         <v>260</v>
       </c>
-      <c r="J101">
-        <v>16</v>
+      <c r="J101" s="8">
+        <v>17</v>
       </c>
       <c r="K101">
         <v>1452</v>
       </c>
-    </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O101" s="6"/>
+    </row>
+    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>16</v>
       </c>
@@ -4585,14 +4684,15 @@
       <c r="I102">
         <v>255</v>
       </c>
-      <c r="J102">
-        <v>15</v>
+      <c r="J102" s="8">
+        <v>16</v>
       </c>
       <c r="K102">
         <v>1617</v>
       </c>
-    </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O102" s="6"/>
+    </row>
+    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>16</v>
       </c>
@@ -4620,14 +4720,15 @@
       <c r="I103">
         <v>261</v>
       </c>
-      <c r="J103">
-        <v>18</v>
+      <c r="J103" s="8">
+        <v>19</v>
       </c>
       <c r="K103">
         <v>1201</v>
       </c>
-    </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O103" s="6"/>
+    </row>
+    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>16</v>
       </c>
@@ -4655,14 +4756,15 @@
       <c r="I104">
         <v>258</v>
       </c>
-      <c r="J104">
-        <v>13</v>
+      <c r="J104" s="8">
+        <v>14</v>
       </c>
       <c r="K104">
         <v>1296</v>
       </c>
-    </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O104" s="6"/>
+    </row>
+    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>16</v>
       </c>
@@ -4690,14 +4792,15 @@
       <c r="I105">
         <v>256</v>
       </c>
-      <c r="J105">
-        <v>17</v>
+      <c r="J105" s="8">
+        <v>18</v>
       </c>
       <c r="K105">
         <v>1452</v>
       </c>
-    </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O105" s="6"/>
+    </row>
+    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>16</v>
       </c>
@@ -4725,14 +4828,15 @@
       <c r="I106">
         <v>259</v>
       </c>
-      <c r="J106">
-        <v>19</v>
+      <c r="J106" s="8">
+        <v>20</v>
       </c>
       <c r="K106">
         <v>1488</v>
       </c>
-    </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O106" s="6"/>
+    </row>
+    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>16</v>
       </c>
@@ -4760,14 +4864,15 @@
       <c r="I107">
         <v>256</v>
       </c>
-      <c r="J107">
-        <v>13</v>
+      <c r="J107" s="8">
+        <v>14</v>
       </c>
       <c r="K107">
         <v>1492</v>
       </c>
-    </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O107" s="6"/>
+    </row>
+    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>16</v>
       </c>
@@ -4795,14 +4900,15 @@
       <c r="I108">
         <v>266</v>
       </c>
-      <c r="J108">
-        <v>25</v>
+      <c r="J108" s="8">
+        <v>26</v>
       </c>
       <c r="K108">
         <v>1474</v>
       </c>
-    </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O108" s="6"/>
+    </row>
+    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>16</v>
       </c>
@@ -4830,14 +4936,15 @@
       <c r="I109">
         <v>261</v>
       </c>
-      <c r="J109">
-        <v>23</v>
+      <c r="J109" s="8">
+        <v>24</v>
       </c>
       <c r="K109">
         <v>1349</v>
       </c>
-    </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O109" s="6"/>
+    </row>
+    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>16</v>
       </c>
@@ -4865,14 +4972,15 @@
       <c r="I110">
         <v>257</v>
       </c>
-      <c r="J110">
-        <v>20</v>
+      <c r="J110" s="8">
+        <v>21</v>
       </c>
       <c r="K110">
         <v>1454</v>
       </c>
-    </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O110" s="6"/>
+    </row>
+    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>16</v>
       </c>
@@ -4900,14 +5008,15 @@
       <c r="I111">
         <v>254</v>
       </c>
-      <c r="J111">
-        <v>16</v>
+      <c r="J111" s="8">
+        <v>17</v>
       </c>
       <c r="K111">
         <v>1310</v>
       </c>
-    </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O111" s="6"/>
+    </row>
+    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>16</v>
       </c>
@@ -4935,14 +5044,15 @@
       <c r="I112">
         <v>250</v>
       </c>
-      <c r="J112">
-        <v>11</v>
+      <c r="J112" s="8">
+        <v>12</v>
       </c>
       <c r="K112">
         <v>1458</v>
       </c>
-    </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O112" s="6"/>
+    </row>
+    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>16</v>
       </c>
@@ -4970,14 +5080,15 @@
       <c r="I113">
         <v>252</v>
       </c>
-      <c r="J113">
-        <v>17</v>
+      <c r="J113" s="8">
+        <v>18</v>
       </c>
       <c r="K113">
         <v>1339</v>
       </c>
-    </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O113" s="6"/>
+    </row>
+    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>16</v>
       </c>
@@ -5005,14 +5116,15 @@
       <c r="I114">
         <v>247</v>
       </c>
-      <c r="J114">
-        <v>10</v>
+      <c r="J114" s="8">
+        <v>11</v>
       </c>
       <c r="K114">
         <v>1486</v>
       </c>
-    </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O114" s="6"/>
+    </row>
+    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>16</v>
       </c>
@@ -5040,14 +5152,15 @@
       <c r="I115">
         <v>257</v>
       </c>
-      <c r="J115">
-        <v>20</v>
+      <c r="J115" s="8">
+        <v>21</v>
       </c>
       <c r="K115">
         <v>1350</v>
       </c>
-    </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O115" s="6"/>
+    </row>
+    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>16</v>
       </c>
@@ -5077,14 +5190,15 @@
         <f>F116-DATE(YEAR(F116),1,1)+1</f>
         <v>257</v>
       </c>
-      <c r="J116">
-        <v>15</v>
+      <c r="J116" s="8">
+        <v>16</v>
       </c>
       <c r="K116">
         <v>1465</v>
       </c>
-    </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O116" s="6"/>
+    </row>
+    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>16</v>
       </c>
@@ -5112,14 +5226,15 @@
       <c r="I117">
         <v>256</v>
       </c>
-      <c r="J117">
-        <v>20</v>
+      <c r="J117" s="8">
+        <v>21</v>
       </c>
       <c r="K117">
         <v>1415</v>
       </c>
-    </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O117" s="6"/>
+    </row>
+    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>16</v>
       </c>
@@ -5147,14 +5262,15 @@
       <c r="I118">
         <v>256</v>
       </c>
-      <c r="J118">
-        <v>18</v>
+      <c r="J118" s="8">
+        <v>19</v>
       </c>
       <c r="K118">
         <v>1658</v>
       </c>
-    </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O118" s="6"/>
+    </row>
+    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>16</v>
       </c>
@@ -5182,14 +5298,15 @@
       <c r="I119">
         <v>259</v>
       </c>
-      <c r="J119">
-        <v>18</v>
+      <c r="J119" s="8">
+        <v>19</v>
       </c>
       <c r="K119">
         <v>1292</v>
       </c>
-    </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O119" s="6"/>
+    </row>
+    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>16</v>
       </c>
@@ -5217,14 +5334,15 @@
       <c r="I120">
         <v>258</v>
       </c>
-      <c r="J120">
-        <v>25</v>
+      <c r="J120" s="8">
+        <v>26</v>
       </c>
       <c r="K120">
         <v>1772</v>
       </c>
-    </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O120" s="6"/>
+    </row>
+    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>16</v>
       </c>
@@ -5252,14 +5370,15 @@
       <c r="I121">
         <v>262</v>
       </c>
-      <c r="J121">
-        <v>23</v>
+      <c r="J121" s="8">
+        <v>24</v>
       </c>
       <c r="K121">
         <v>1298</v>
       </c>
-    </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O121" s="6"/>
+    </row>
+    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>16</v>
       </c>
@@ -5287,14 +5406,15 @@
       <c r="I122">
         <v>254</v>
       </c>
-      <c r="J122">
-        <v>14</v>
+      <c r="J122" s="8">
+        <v>15</v>
       </c>
       <c r="K122">
         <v>1661</v>
       </c>
-    </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O122" s="6"/>
+    </row>
+    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>16</v>
       </c>
@@ -5322,14 +5442,15 @@
       <c r="I123">
         <v>260</v>
       </c>
-      <c r="J123">
-        <v>19</v>
+      <c r="J123" s="8">
+        <v>20</v>
       </c>
       <c r="K123">
         <v>1183</v>
       </c>
-    </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O123" s="6"/>
+    </row>
+    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>16</v>
       </c>
@@ -5357,14 +5478,15 @@
       <c r="I124">
         <v>260</v>
       </c>
-      <c r="J124">
-        <v>21</v>
+      <c r="J124" s="8">
+        <v>22</v>
       </c>
       <c r="K124">
         <v>1379</v>
       </c>
-    </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O124" s="6"/>
+    </row>
+    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>16</v>
       </c>
@@ -5392,14 +5514,15 @@
       <c r="I125">
         <v>253</v>
       </c>
-      <c r="J125">
-        <v>16</v>
+      <c r="J125" s="8">
+        <v>17</v>
       </c>
       <c r="K125">
         <v>1188</v>
       </c>
-    </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O125" s="6"/>
+    </row>
+    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>17</v>
       </c>
@@ -5427,8 +5550,8 @@
       <c r="I126">
         <v>208</v>
       </c>
-      <c r="J126">
-        <v>14</v>
+      <c r="J126" s="8">
+        <v>15</v>
       </c>
       <c r="K126">
         <v>1882</v>
@@ -5436,8 +5559,9 @@
       <c r="M126">
         <v>1</v>
       </c>
-    </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O126" s="6"/>
+    </row>
+    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>17</v>
       </c>
@@ -5465,7 +5589,7 @@
       <c r="I127" s="2">
         <v>218</v>
       </c>
-      <c r="J127" s="4">
+      <c r="J127" s="7">
         <v>22</v>
       </c>
       <c r="K127">
@@ -5474,8 +5598,9 @@
       <c r="M127">
         <v>1</v>
       </c>
-    </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O127" s="6"/>
+    </row>
+    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>17</v>
       </c>
@@ -5503,14 +5628,15 @@
       <c r="I128">
         <v>224</v>
       </c>
-      <c r="J128">
-        <v>24</v>
+      <c r="J128" s="8">
+        <v>25</v>
       </c>
       <c r="K128">
         <v>1915</v>
       </c>
-    </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O128" s="6"/>
+    </row>
+    <row r="129" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>17</v>
       </c>
@@ -5538,14 +5664,15 @@
       <c r="I129">
         <v>220</v>
       </c>
-      <c r="J129">
-        <v>22</v>
+      <c r="J129" s="8">
+        <v>23</v>
       </c>
       <c r="K129">
         <v>1905</v>
       </c>
-    </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O129" s="6"/>
+    </row>
+    <row r="130" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>17</v>
       </c>
@@ -5573,14 +5700,15 @@
       <c r="I130">
         <v>225</v>
       </c>
-      <c r="J130">
-        <v>32</v>
+      <c r="J130" s="8">
+        <v>33</v>
       </c>
       <c r="K130">
         <v>1647</v>
       </c>
-    </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O130" s="6"/>
+    </row>
+    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>17</v>
       </c>
@@ -5608,14 +5736,15 @@
       <c r="I131">
         <v>238</v>
       </c>
-      <c r="J131">
-        <v>35</v>
+      <c r="J131" s="8">
+        <v>36</v>
       </c>
       <c r="K131">
         <v>1433</v>
       </c>
-    </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O131" s="6"/>
+    </row>
+    <row r="132" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>17</v>
       </c>
@@ -5643,14 +5772,15 @@
       <c r="I132">
         <v>219</v>
       </c>
-      <c r="J132">
-        <v>22</v>
+      <c r="J132" s="8">
+        <v>23</v>
       </c>
       <c r="K132">
         <v>1746</v>
       </c>
-    </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O132" s="6"/>
+    </row>
+    <row r="133" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>17</v>
       </c>
@@ -5678,14 +5808,15 @@
       <c r="I133">
         <v>223</v>
       </c>
-      <c r="J133">
-        <v>21</v>
+      <c r="J133" s="8">
+        <v>22</v>
       </c>
       <c r="K133">
         <v>1742</v>
       </c>
-    </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O133" s="6"/>
+    </row>
+    <row r="134" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>17</v>
       </c>
@@ -5713,14 +5844,15 @@
       <c r="I134">
         <v>234</v>
       </c>
-      <c r="J134">
-        <v>38</v>
+      <c r="J134" s="8">
+        <v>39</v>
       </c>
       <c r="K134">
         <v>1649</v>
       </c>
-    </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O134" s="6"/>
+    </row>
+    <row r="135" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>17</v>
       </c>
@@ -5748,14 +5880,15 @@
       <c r="I135">
         <v>226</v>
       </c>
-      <c r="J135">
-        <v>25</v>
+      <c r="J135" s="8">
+        <v>26</v>
       </c>
       <c r="K135">
         <v>1600</v>
       </c>
-    </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O135" s="6"/>
+    </row>
+    <row r="136" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>17</v>
       </c>
@@ -5783,14 +5916,15 @@
       <c r="I136">
         <v>239</v>
       </c>
-      <c r="J136">
-        <v>35</v>
+      <c r="J136" s="8">
+        <v>36</v>
       </c>
       <c r="K136">
         <v>1533</v>
       </c>
-    </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O136" s="6"/>
+    </row>
+    <row r="137" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>17</v>
       </c>
@@ -5818,14 +5952,15 @@
       <c r="I137">
         <v>233</v>
       </c>
-      <c r="J137">
-        <v>30</v>
+      <c r="J137" s="8">
+        <v>31</v>
       </c>
       <c r="K137">
         <v>1703</v>
       </c>
-    </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O137" s="6"/>
+    </row>
+    <row r="138" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>17</v>
       </c>
@@ -5853,14 +5988,15 @@
       <c r="I138">
         <v>232</v>
       </c>
-      <c r="J138">
-        <v>28</v>
+      <c r="J138" s="8">
+        <v>29</v>
       </c>
       <c r="K138">
         <v>1518</v>
       </c>
-    </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O138" s="6"/>
+    </row>
+    <row r="139" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>17</v>
       </c>
@@ -5888,14 +6024,15 @@
       <c r="I139">
         <v>222</v>
       </c>
-      <c r="J139">
-        <v>19</v>
+      <c r="J139" s="8">
+        <v>20</v>
       </c>
       <c r="K139">
         <v>1718</v>
       </c>
-    </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O139" s="6"/>
+    </row>
+    <row r="140" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>17</v>
       </c>
@@ -5923,14 +6060,15 @@
       <c r="I140">
         <v>228</v>
       </c>
-      <c r="J140">
-        <v>22</v>
+      <c r="J140" s="8">
+        <v>23</v>
       </c>
       <c r="K140">
         <v>1722</v>
       </c>
-    </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O140" s="6"/>
+    </row>
+    <row r="141" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>17</v>
       </c>
@@ -5958,14 +6096,15 @@
       <c r="I141">
         <v>219</v>
       </c>
-      <c r="J141">
-        <v>14</v>
+      <c r="J141" s="8">
+        <v>15</v>
       </c>
       <c r="K141">
         <v>1820</v>
       </c>
-    </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O141" s="6"/>
+    </row>
+    <row r="142" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>17</v>
       </c>
@@ -5993,14 +6132,15 @@
       <c r="I142">
         <v>233</v>
       </c>
-      <c r="J142">
-        <v>31</v>
+      <c r="J142" s="8">
+        <v>32</v>
       </c>
       <c r="K142">
         <v>1711</v>
       </c>
-    </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O142" s="6"/>
+    </row>
+    <row r="143" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>17</v>
       </c>
@@ -6028,14 +6168,15 @@
       <c r="I143">
         <v>230</v>
       </c>
-      <c r="J143">
-        <v>26</v>
+      <c r="J143" s="8">
+        <v>27</v>
       </c>
       <c r="K143">
         <v>1747</v>
       </c>
-    </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O143" s="6"/>
+    </row>
+    <row r="144" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>17</v>
       </c>
@@ -6063,14 +6204,15 @@
       <c r="I144">
         <v>231</v>
       </c>
-      <c r="J144">
-        <v>24</v>
+      <c r="J144" s="8">
+        <v>25</v>
       </c>
       <c r="K144">
         <v>1630</v>
       </c>
-    </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O144" s="6"/>
+    </row>
+    <row r="145" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>17</v>
       </c>
@@ -6098,14 +6240,15 @@
       <c r="I145">
         <v>231</v>
       </c>
-      <c r="J145">
-        <v>24</v>
+      <c r="J145" s="8">
+        <v>25</v>
       </c>
       <c r="K145">
         <v>1633</v>
       </c>
-    </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O145" s="6"/>
+    </row>
+    <row r="146" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>17</v>
       </c>
@@ -6133,14 +6276,15 @@
       <c r="I146">
         <v>227</v>
       </c>
-      <c r="J146">
-        <v>26</v>
+      <c r="J146" s="8">
+        <v>27</v>
       </c>
       <c r="K146">
         <v>1662</v>
       </c>
-    </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O146" s="6"/>
+    </row>
+    <row r="147" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>17</v>
       </c>
@@ -6168,14 +6312,15 @@
       <c r="I147">
         <v>228</v>
       </c>
-      <c r="J147">
-        <v>25</v>
+      <c r="J147" s="8">
+        <v>26</v>
       </c>
       <c r="K147">
         <v>1608</v>
       </c>
-    </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O147" s="6"/>
+    </row>
+    <row r="148" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>17</v>
       </c>
@@ -6203,14 +6348,15 @@
       <c r="I148">
         <v>224</v>
       </c>
-      <c r="J148">
-        <v>22</v>
+      <c r="J148" s="8">
+        <v>23</v>
       </c>
       <c r="K148">
         <v>1752</v>
       </c>
-    </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O148" s="6"/>
+    </row>
+    <row r="149" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>17</v>
       </c>
@@ -6238,14 +6384,15 @@
       <c r="I149">
         <v>230</v>
       </c>
-      <c r="J149">
-        <v>22</v>
+      <c r="J149" s="8">
+        <v>23</v>
       </c>
       <c r="K149">
         <v>1603</v>
       </c>
-    </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O149" s="6"/>
+    </row>
+    <row r="150" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>17</v>
       </c>
@@ -6273,14 +6420,15 @@
       <c r="I150">
         <v>236</v>
       </c>
-      <c r="J150">
-        <v>27</v>
+      <c r="J150" s="8">
+        <v>28</v>
       </c>
       <c r="K150">
         <v>1587</v>
       </c>
-    </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O150" s="6"/>
+    </row>
+    <row r="151" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>17</v>
       </c>
@@ -6308,14 +6456,15 @@
       <c r="I151">
         <v>236</v>
       </c>
-      <c r="J151">
-        <v>31</v>
+      <c r="J151" s="8">
+        <v>32</v>
       </c>
       <c r="K151">
         <v>1718</v>
       </c>
-    </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O151" s="6"/>
+    </row>
+    <row r="152" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>17</v>
       </c>
@@ -6343,14 +6492,15 @@
       <c r="I152">
         <v>232</v>
       </c>
-      <c r="J152">
-        <v>28</v>
+      <c r="J152" s="8">
+        <v>29</v>
       </c>
       <c r="K152">
         <v>1717</v>
       </c>
-    </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O152" s="6"/>
+    </row>
+    <row r="153" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>17</v>
       </c>
@@ -6378,14 +6528,15 @@
       <c r="I153">
         <v>234</v>
       </c>
-      <c r="J153">
-        <v>24</v>
+      <c r="J153" s="8">
+        <v>25</v>
       </c>
       <c r="K153">
         <v>1644</v>
       </c>
-    </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O153" s="6"/>
+    </row>
+    <row r="154" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>17</v>
       </c>
@@ -6413,14 +6564,15 @@
       <c r="I154">
         <v>237</v>
       </c>
-      <c r="J154">
-        <v>29</v>
+      <c r="J154" s="8">
+        <v>30</v>
       </c>
       <c r="K154">
         <v>1508</v>
       </c>
-    </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O154" s="6"/>
+    </row>
+    <row r="155" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>17</v>
       </c>
@@ -6448,14 +6600,15 @@
       <c r="I155">
         <v>231</v>
       </c>
-      <c r="J155">
-        <v>24</v>
+      <c r="J155" s="8">
+        <v>26</v>
       </c>
       <c r="K155">
         <v>1642</v>
       </c>
-    </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O155" s="6"/>
+    </row>
+    <row r="156" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>17</v>
       </c>
@@ -6483,14 +6636,15 @@
       <c r="I156">
         <v>231</v>
       </c>
-      <c r="J156">
-        <v>24</v>
+      <c r="J156" s="8">
+        <v>25</v>
       </c>
       <c r="K156">
         <v>1607</v>
       </c>
-    </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O156" s="6"/>
+    </row>
+    <row r="157" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>17</v>
       </c>
@@ -6518,14 +6672,15 @@
       <c r="I157">
         <v>235</v>
       </c>
-      <c r="J157">
-        <v>20</v>
+      <c r="J157" s="8">
+        <v>21</v>
       </c>
       <c r="K157">
         <v>1739</v>
       </c>
-    </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O157" s="6"/>
+    </row>
+    <row r="158" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>17</v>
       </c>
@@ -6553,14 +6708,15 @@
       <c r="I158">
         <v>234</v>
       </c>
-      <c r="J158">
-        <v>22</v>
+      <c r="J158" s="8">
+        <v>23</v>
       </c>
       <c r="K158">
         <v>1523</v>
       </c>
-    </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O158" s="6"/>
+    </row>
+    <row r="159" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>17</v>
       </c>
@@ -6588,14 +6744,15 @@
       <c r="I159">
         <v>232</v>
       </c>
-      <c r="J159">
-        <v>22</v>
+      <c r="J159" s="8">
+        <v>23</v>
       </c>
       <c r="K159">
         <v>1638</v>
       </c>
-    </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O159" s="6"/>
+    </row>
+    <row r="160" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>17</v>
       </c>
@@ -6623,14 +6780,15 @@
       <c r="I160">
         <v>234</v>
       </c>
-      <c r="J160">
-        <v>26</v>
+      <c r="J160" s="8">
+        <v>27</v>
       </c>
       <c r="K160">
         <v>1505</v>
       </c>
-    </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O160" s="6"/>
+    </row>
+    <row r="161" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>17</v>
       </c>
@@ -6658,14 +6816,15 @@
       <c r="I161">
         <v>236</v>
       </c>
-      <c r="J161">
-        <v>27</v>
+      <c r="J161" s="8">
+        <v>28</v>
       </c>
       <c r="K161">
         <v>1814</v>
       </c>
-    </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O161" s="6"/>
+    </row>
+    <row r="162" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>17</v>
       </c>
@@ -6693,14 +6852,15 @@
       <c r="I162">
         <v>234</v>
       </c>
-      <c r="J162">
-        <v>22</v>
+      <c r="J162" s="8">
+        <v>23</v>
       </c>
       <c r="K162">
         <v>1684</v>
       </c>
-    </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O162" s="6"/>
+    </row>
+    <row r="163" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>17</v>
       </c>
@@ -6728,14 +6888,15 @@
       <c r="I163">
         <v>235</v>
       </c>
-      <c r="J163">
-        <v>27</v>
+      <c r="J163" s="8">
+        <v>28</v>
       </c>
       <c r="K163">
         <v>1796</v>
       </c>
-    </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O163" s="6"/>
+    </row>
+    <row r="164" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>17</v>
       </c>
@@ -6763,14 +6924,15 @@
       <c r="I164">
         <v>235</v>
       </c>
-      <c r="J164">
-        <v>25</v>
+      <c r="J164" s="8">
+        <v>26</v>
       </c>
       <c r="K164">
         <v>1725</v>
       </c>
-    </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O164" s="6"/>
+    </row>
+    <row r="165" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>17</v>
       </c>
@@ -6798,14 +6960,15 @@
       <c r="I165">
         <v>237</v>
       </c>
-      <c r="J165">
-        <v>21</v>
+      <c r="J165" s="8">
+        <v>22</v>
       </c>
       <c r="K165">
         <v>1641</v>
       </c>
-    </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O165" s="6"/>
+    </row>
+    <row r="166" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>17</v>
       </c>
@@ -6833,14 +6996,15 @@
       <c r="I166">
         <v>242</v>
       </c>
-      <c r="J166">
-        <v>28</v>
+      <c r="J166" s="8">
+        <v>29</v>
       </c>
       <c r="K166">
         <v>1495</v>
       </c>
-    </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O166" s="6"/>
+    </row>
+    <row r="167" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J167" s="6"/>
     </row>
   </sheetData>

</xml_diff>